<commit_message>
Add Template for all project
</commit_message>
<xml_diff>
--- a/Testcase Generate from Gitlab/input/Testcase-template.xlsx
+++ b/Testcase Generate from Gitlab/input/Testcase-template.xlsx
@@ -93,13 +93,13 @@
     <t>Site is Opened</t>
   </si>
   <si>
-    <t>Passed</t>
-  </si>
-  <si>
     <t>Test PR - Status change</t>
   </si>
   <si>
     <t>Today</t>
+  </si>
+  <si>
+    <t>Pass</t>
   </si>
 </sst>
 </file>
@@ -319,27 +319,60 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
@@ -355,47 +388,14 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -680,8 +680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -692,19 +692,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="26"/>
+      <c r="B1" s="15"/>
       <c r="C1" s="1">
         <v>43</v>
       </c>
-      <c r="D1" s="30" t="s">
+      <c r="D1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="26"/>
+      <c r="E1" s="15"/>
       <c r="F1" s="16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G1" s="16"/>
       <c r="H1" s="16"/>
@@ -713,29 +713,29 @@
       <c r="K1" s="17"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="26"/>
+      <c r="B2" s="15"/>
       <c r="C2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="30" t="s">
+      <c r="D2" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="26"/>
+      <c r="E2" s="15"/>
       <c r="F2" s="16" t="s">
         <v>19</v>
       </c>
       <c r="G2" s="17"/>
-      <c r="H2" s="33" t="s">
+      <c r="H2" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="26"/>
-      <c r="J2" s="34" t="s">
+      <c r="I2" s="15"/>
+      <c r="J2" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="K2" s="35"/>
+      <c r="K2" s="20"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
@@ -751,10 +751,10 @@
       <c r="K3" s="4"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="36" t="s">
+      <c r="A4" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="37"/>
+      <c r="B4" s="22"/>
       <c r="C4" s="10"/>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
@@ -779,27 +779,27 @@
       <c r="K5" s="4"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="33" t="s">
+      <c r="A6" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="37"/>
+      <c r="B6" s="22"/>
       <c r="C6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="33" t="s">
+      <c r="D6" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="37"/>
-      <c r="F6" s="38" t="s">
-        <v>26</v>
-      </c>
-      <c r="G6" s="39"/>
-      <c r="H6" s="33" t="s">
+      <c r="E6" s="22"/>
+      <c r="F6" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="24"/>
+      <c r="H6" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="I6" s="37"/>
-      <c r="J6" s="32"/>
-      <c r="K6" s="32"/>
+      <c r="I6" s="22"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="6"/>
@@ -818,37 +818,37 @@
       <c r="A8" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="28" t="s">
+      <c r="B8" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="29"/>
-      <c r="D8" s="29"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="26"/>
       <c r="E8" s="7"/>
       <c r="F8" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="G8" s="30" t="s">
+      <c r="G8" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="H8" s="31"/>
-      <c r="I8" s="31"/>
-      <c r="J8" s="31"/>
-      <c r="K8" s="31"/>
+      <c r="H8" s="27"/>
+      <c r="I8" s="27"/>
+      <c r="J8" s="27"/>
+      <c r="K8" s="27"/>
     </row>
     <row r="9" spans="1:11" ht="13" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="8">
         <v>1</v>
       </c>
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="19"/>
-      <c r="D9" s="20"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="30"/>
       <c r="E9" s="3"/>
       <c r="F9" s="8">
         <v>1</v>
       </c>
-      <c r="G9" s="15"/>
+      <c r="G9" s="31"/>
       <c r="H9" s="16"/>
       <c r="I9" s="16"/>
       <c r="J9" s="16"/>
@@ -858,12 +858,12 @@
       <c r="A10" s="8">
         <v>2</v>
       </c>
-      <c r="B10" s="18"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="20"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="30"/>
       <c r="E10" s="3"/>
       <c r="F10" s="8"/>
-      <c r="G10" s="15"/>
+      <c r="G10" s="31"/>
       <c r="H10" s="16"/>
       <c r="I10" s="16"/>
       <c r="J10" s="16"/>
@@ -873,12 +873,12 @@
       <c r="A11" s="8">
         <v>3</v>
       </c>
-      <c r="B11" s="18"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="20"/>
+      <c r="B11" s="28"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="30"/>
       <c r="E11" s="3"/>
       <c r="F11" s="8"/>
-      <c r="G11" s="15"/>
+      <c r="G11" s="31"/>
       <c r="H11" s="16"/>
       <c r="I11" s="16"/>
       <c r="J11" s="16"/>
@@ -888,12 +888,12 @@
       <c r="A12" s="8">
         <v>4</v>
       </c>
-      <c r="B12" s="18"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="20"/>
+      <c r="B12" s="28"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="30"/>
       <c r="E12" s="3"/>
       <c r="F12" s="8"/>
-      <c r="G12" s="15"/>
+      <c r="G12" s="31"/>
       <c r="H12" s="16"/>
       <c r="I12" s="16"/>
       <c r="J12" s="16"/>
@@ -928,66 +928,85 @@
       <c r="K14" s="4"/>
     </row>
     <row r="16" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="21" t="s">
+      <c r="A16" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="B16" s="21" t="s">
+      <c r="B16" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="22"/>
-      <c r="D16" s="24" t="s">
+      <c r="C16" s="33"/>
+      <c r="D16" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="E16" s="25"/>
-      <c r="F16" s="21" t="s">
+      <c r="E16" s="36"/>
+      <c r="F16" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="G16" s="27"/>
-      <c r="H16" s="27"/>
-      <c r="I16" s="21" t="s">
+      <c r="G16" s="37"/>
+      <c r="H16" s="37"/>
+      <c r="I16" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="J16" s="27"/>
-      <c r="K16" s="27"/>
+      <c r="J16" s="37"/>
+      <c r="K16" s="37"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A17" s="22"/>
-      <c r="B17" s="23"/>
-      <c r="C17" s="23"/>
-      <c r="D17" s="26"/>
-      <c r="E17" s="26"/>
-      <c r="F17" s="27"/>
-      <c r="G17" s="27"/>
-      <c r="H17" s="27"/>
-      <c r="I17" s="27"/>
-      <c r="J17" s="27"/>
-      <c r="K17" s="27"/>
+      <c r="A17" s="33"/>
+      <c r="B17" s="34"/>
+      <c r="C17" s="34"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="37"/>
+      <c r="G17" s="37"/>
+      <c r="H17" s="37"/>
+      <c r="I17" s="37"/>
+      <c r="J17" s="37"/>
+      <c r="K17" s="37"/>
     </row>
     <row r="18" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="8">
         <v>1</v>
       </c>
-      <c r="B18" s="13" t="s">
+      <c r="B18" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="C18" s="14"/>
-      <c r="D18" s="13" t="s">
+      <c r="C18" s="39"/>
+      <c r="D18" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="E18" s="13"/>
-      <c r="F18" s="15" t="s">
+      <c r="E18" s="38"/>
+      <c r="F18" s="31" t="s">
         <v>23</v>
       </c>
       <c r="G18" s="16"/>
       <c r="H18" s="17"/>
-      <c r="I18" s="15" t="s">
-        <v>24</v>
+      <c r="I18" s="31" t="s">
+        <v>26</v>
       </c>
       <c r="J18" s="16"/>
       <c r="K18" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="G11:K11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="G12:K12"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="I18:K18"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B16:C17"/>
+    <mergeCell ref="D16:E17"/>
+    <mergeCell ref="F16:H17"/>
+    <mergeCell ref="I16:K17"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="G8:K8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="G9:K9"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="G10:K10"/>
     <mergeCell ref="J6:K6"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="D1:E1"/>
@@ -1002,25 +1021,6 @@
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="F6:G6"/>
     <mergeCell ref="H6:I6"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="G8:K8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="G9:K9"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="G10:K10"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B16:C17"/>
-    <mergeCell ref="D16:E17"/>
-    <mergeCell ref="F16:H17"/>
-    <mergeCell ref="I16:K17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="F18:H18"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="G11:K11"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="G12:K12"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="I18:K18"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>

</xml_diff>